<commit_message>
Reorganised Codebooks and City Fixer Code
</commit_message>
<xml_diff>
--- a/AP_Youth_Survey_Codebook.xlsx
+++ b/AP_Youth_Survey_Codebook.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vaibhav/Documents/CPR - Work/AP Project/survey-responses-AP-/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C13AA16-178B-054B-94FB-9D1FEBC7797F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60BA68FE-9833-3240-9ECB-0A60B6826A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Main_Survey" sheetId="1" r:id="rId1"/>
+    <sheet name="Household_Roster" sheetId="2" r:id="rId2"/>
+    <sheet name="Outmigration_Roster" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="494">
   <si>
     <t>start</t>
   </si>
@@ -1287,6 +1289,231 @@
   </si>
   <si>
     <t>Y_G_189</t>
+  </si>
+  <si>
+    <t>SNo</t>
+  </si>
+  <si>
+    <t>Household Roster</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Relationship to the Youth Respondent</t>
+  </si>
+  <si>
+    <t>H_1</t>
+  </si>
+  <si>
+    <t>Is this person a schoolgoing child between class 1 and class 12?</t>
+  </si>
+  <si>
+    <t>H_2</t>
+  </si>
+  <si>
+    <t>If yes, then what class (mark 0 for pre-school or anything below Class-I)?</t>
+  </si>
+  <si>
+    <t>H_3</t>
+  </si>
+  <si>
+    <t>Marital Status</t>
+  </si>
+  <si>
+    <t>H_4</t>
+  </si>
+  <si>
+    <t>Completed Level of Education Attained</t>
+  </si>
+  <si>
+    <t>H_5</t>
+  </si>
+  <si>
+    <t>Primary Activity</t>
+  </si>
+  <si>
+    <t>H_6</t>
+  </si>
+  <si>
+    <t>Others (specify)</t>
+  </si>
+  <si>
+    <t>H_7</t>
+  </si>
+  <si>
+    <t>Sector of Job</t>
+  </si>
+  <si>
+    <t>H_8</t>
+  </si>
+  <si>
+    <t>Description of Sector</t>
+  </si>
+  <si>
+    <t>H_9</t>
+  </si>
+  <si>
+    <t>Occupational Categories</t>
+  </si>
+  <si>
+    <t>H_10</t>
+  </si>
+  <si>
+    <t>Description of Occupation</t>
+  </si>
+  <si>
+    <t>H_11</t>
+  </si>
+  <si>
+    <t>Nature of Employer</t>
+  </si>
+  <si>
+    <t>H_12</t>
+  </si>
+  <si>
+    <t>Does this person have a phone in her/his name?</t>
+  </si>
+  <si>
+    <t>H_13</t>
+  </si>
+  <si>
+    <t>Is it a smartphone?</t>
+  </si>
+  <si>
+    <t>H_14</t>
+  </si>
+  <si>
+    <t>Does this person have an Aadhar card?</t>
+  </si>
+  <si>
+    <t>H_15</t>
+  </si>
+  <si>
+    <t>Kind of School Attended</t>
+  </si>
+  <si>
+    <t>H_16</t>
+  </si>
+  <si>
+    <t>Other (please specify)...21</t>
+  </si>
+  <si>
+    <t>H_17</t>
+  </si>
+  <si>
+    <t>Medium of Instruction</t>
+  </si>
+  <si>
+    <t>H_18</t>
+  </si>
+  <si>
+    <t>Other (please specify)...23</t>
+  </si>
+  <si>
+    <t>H_19</t>
+  </si>
+  <si>
+    <t>What is the board of the school?</t>
+  </si>
+  <si>
+    <t>H_20</t>
+  </si>
+  <si>
+    <t>Other (please specify)...25</t>
+  </si>
+  <si>
+    <t>H_21</t>
+  </si>
+  <si>
+    <t>What are annual fees paid to the school (including school fees, uniform fees, etc.) in rupees?</t>
+  </si>
+  <si>
+    <t>H_22</t>
+  </si>
+  <si>
+    <t>What are annual fees paid for education of this child outside of school (including private tuitions) in rupees?</t>
+  </si>
+  <si>
+    <t>H_23</t>
+  </si>
+  <si>
+    <t>–</t>
+  </si>
+  <si>
+    <t>_parent_table_name</t>
+  </si>
+  <si>
+    <t>_parent_index</t>
+  </si>
+  <si>
+    <t>_submission__id</t>
+  </si>
+  <si>
+    <t>_submission__uuid</t>
+  </si>
+  <si>
+    <t>_submission__submission_time</t>
+  </si>
+  <si>
+    <t>_submission__validation_status</t>
+  </si>
+  <si>
+    <t>_submission__notes</t>
+  </si>
+  <si>
+    <t>_submission__status</t>
+  </si>
+  <si>
+    <t>_submission__submitted_by</t>
+  </si>
+  <si>
+    <t>_submission__tags</t>
+  </si>
+  <si>
+    <t>Outmigration Roster</t>
+  </si>
+  <si>
+    <t>Relation to Youth Respondent</t>
+  </si>
+  <si>
+    <t>O_1</t>
+  </si>
+  <si>
+    <t>Present Location of the out-migrant</t>
+  </si>
+  <si>
+    <t>O_2</t>
+  </si>
+  <si>
+    <t>Do you receive remittances from that person?</t>
+  </si>
+  <si>
+    <t>O_3</t>
+  </si>
+  <si>
+    <t>If yes, what is the total amount of remittances received in last 365 days (INR)?</t>
+  </si>
+  <si>
+    <t>O_4</t>
+  </si>
+  <si>
+    <t>What is the most important thing you could afford because of the remittances which you could not have afforded otherwise</t>
+  </si>
+  <si>
+    <t>O_5</t>
+  </si>
+  <si>
+    <t>Other (please specify)</t>
+  </si>
+  <si>
+    <t>O_6</t>
   </si>
 </sst>
 </file>
@@ -1336,10 +1563,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1681,7 +1917,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D214"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -1716,7 +1952,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="str">
-        <f>A2</f>
+        <f t="shared" ref="D2:D13" si="0">A2</f>
         <v>start</v>
       </c>
     </row>
@@ -1728,7 +1964,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="str">
-        <f>A3</f>
+        <f t="shared" si="0"/>
         <v>end</v>
       </c>
     </row>
@@ -1740,7 +1976,7 @@
         <v>4</v>
       </c>
       <c r="D4" t="str">
-        <f>A4</f>
+        <f t="shared" si="0"/>
         <v>deviceid</v>
       </c>
     </row>
@@ -1752,7 +1988,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="str">
-        <f>A5</f>
+        <f t="shared" si="0"/>
         <v>audit</v>
       </c>
     </row>
@@ -1764,7 +2000,7 @@
         <v>4</v>
       </c>
       <c r="D6" t="str">
-        <f>A6</f>
+        <f t="shared" si="0"/>
         <v>audit_URL</v>
       </c>
     </row>
@@ -1779,7 +2015,7 @@
         <v>221</v>
       </c>
       <c r="D7" t="str">
-        <f>A7</f>
+        <f t="shared" si="0"/>
         <v>Enumerator Code</v>
       </c>
     </row>
@@ -1794,7 +2030,7 @@
         <v>221</v>
       </c>
       <c r="D8" t="str">
-        <f>A8</f>
+        <f t="shared" si="0"/>
         <v>Enumerator Name</v>
       </c>
     </row>
@@ -1809,7 +2045,7 @@
         <v>221</v>
       </c>
       <c r="D9" t="str">
-        <f>A9</f>
+        <f t="shared" si="0"/>
         <v>City Code</v>
       </c>
     </row>
@@ -1824,7 +2060,7 @@
         <v>221</v>
       </c>
       <c r="D10" t="str">
-        <f>A10</f>
+        <f t="shared" si="0"/>
         <v>City Name</v>
       </c>
     </row>
@@ -1839,7 +2075,7 @@
         <v>221</v>
       </c>
       <c r="D11" t="str">
-        <f>A11</f>
+        <f t="shared" si="0"/>
         <v>Secretariat Code</v>
       </c>
     </row>
@@ -1854,7 +2090,7 @@
         <v>221</v>
       </c>
       <c r="D12" t="str">
-        <f>A12</f>
+        <f t="shared" si="0"/>
         <v>Secretariat Name</v>
       </c>
     </row>
@@ -1869,7 +2105,7 @@
         <v>221</v>
       </c>
       <c r="D13" t="str">
-        <f>A13</f>
+        <f t="shared" si="0"/>
         <v>Respondent ID</v>
       </c>
     </row>
@@ -4539,7 +4775,7 @@
         <v>4</v>
       </c>
       <c r="D204" t="str">
-        <f t="shared" ref="D204:D214" si="0">A204</f>
+        <f t="shared" ref="D204:D214" si="1">A204</f>
         <v>_version_</v>
       </c>
     </row>
@@ -4551,7 +4787,7 @@
         <v>4</v>
       </c>
       <c r="D205" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>_version__001</v>
       </c>
     </row>
@@ -4563,7 +4799,7 @@
         <v>8</v>
       </c>
       <c r="D206" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>_id</v>
       </c>
     </row>
@@ -4575,7 +4811,7 @@
         <v>4</v>
       </c>
       <c r="D207" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>_uuid</v>
       </c>
     </row>
@@ -4587,7 +4823,7 @@
         <v>1</v>
       </c>
       <c r="D208" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>_submission_time</v>
       </c>
     </row>
@@ -4599,7 +4835,7 @@
         <v>4</v>
       </c>
       <c r="D209" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>_validation_status</v>
       </c>
     </row>
@@ -4611,7 +4847,7 @@
         <v>68</v>
       </c>
       <c r="D210" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>_notes</v>
       </c>
     </row>
@@ -4623,7 +4859,7 @@
         <v>4</v>
       </c>
       <c r="D211" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>_status</v>
       </c>
     </row>
@@ -4635,7 +4871,7 @@
         <v>4</v>
       </c>
       <c r="D212" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>_submitted_by</v>
       </c>
     </row>
@@ -4647,7 +4883,7 @@
         <v>68</v>
       </c>
       <c r="D213" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>_tags</v>
       </c>
     </row>
@@ -4659,7 +4895,7 @@
         <v>8</v>
       </c>
       <c r="D214" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>_index</v>
       </c>
     </row>
@@ -4667,4 +4903,858 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F6040D8-6C0C-3D4B-A4B1-4DD2703FB6C6}">
+  <dimension ref="A1:D39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="29" customWidth="1"/>
+    <col min="2" max="2" width="25.83203125" customWidth="1"/>
+    <col min="3" max="3" width="31.6640625" customWidth="1"/>
+    <col min="4" max="4" width="43.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>444</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>450</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>468</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>470</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>471</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>470</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>472</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>470</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>470</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>470</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>475</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>470</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>470</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>477</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>470</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>478</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>470</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>470</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>480</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>470</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>480</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45D1D7FB-86F8-AF44-A288-BB1B823D6169}">
+  <dimension ref="A1:D19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="33.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>481</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>482</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>481</v>
+      </c>
+      <c r="D3" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>484</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>481</v>
+      </c>
+      <c r="D4" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>481</v>
+      </c>
+      <c r="D5" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="112" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>481</v>
+      </c>
+      <c r="D6" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="176" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>481</v>
+      </c>
+      <c r="D7" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" t="s">
+        <v>481</v>
+      </c>
+      <c r="D8" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>481</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>471</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>481</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>472</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>481</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>481</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>481</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>475</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>481</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" t="s">
+        <v>481</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>477</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" t="s">
+        <v>481</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>478</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>481</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>481</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>480</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" t="s">
+        <v>481</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>480</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>